<commit_message>
TP#20088: Fixed smart post sheet
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/IMPB SmartPost.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/IMPB SmartPost.xlsx
@@ -2110,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4195,7 +4195,7 @@
         <v>85</v>
       </c>
       <c r="E3" s="6">
-        <v>630151821</v>
+        <v>630148367</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
@@ -4317,8 +4317,8 @@
       <c r="D4" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="13">
-        <v>630151821</v>
+      <c r="E4" s="6">
+        <v>630148367</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
@@ -4438,8 +4438,8 @@
       <c r="D5" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="13">
-        <v>630151821</v>
+      <c r="E5" s="6">
+        <v>630148367</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12" t="s">
@@ -4565,8 +4565,8 @@
       <c r="D6" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="13">
-        <v>630151821</v>
+      <c r="E6" s="6">
+        <v>630148367</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12" t="s">
@@ -4688,8 +4688,8 @@
       <c r="D7" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="13">
-        <v>630151821</v>
+      <c r="E7" s="6">
+        <v>630148367</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12" t="s">
@@ -4815,8 +4815,8 @@
       <c r="D8" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="13">
-        <v>630151821</v>
+      <c r="E8" s="6">
+        <v>630148367</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12" t="s">
@@ -4938,8 +4938,8 @@
       <c r="D9" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="13">
-        <v>630151821</v>
+      <c r="E9" s="6">
+        <v>630148367</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12" t="s">
@@ -5063,8 +5063,8 @@
       <c r="D10" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="13">
-        <v>630151821</v>
+      <c r="E10" s="6">
+        <v>630148367</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12" t="s">

</xml_diff>